<commit_message>
Setup initial entities, enums and contracts
</commit_message>
<xml_diff>
--- a/docs/SISTEMAS.xlsx
+++ b/docs/SISTEMAS.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="8" activeTab="15"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="MAPAMUNDI" sheetId="23" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="MAGIA" sheetId="18" r:id="rId15"/>
     <sheet name="INVENTARIO Y EQUIPAMIENTO" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="538">
   <si>
     <t>SISTEMA DE DISTANCIAS Y ÁREAS</t>
   </si>
@@ -1799,11 +1799,17 @@
   <si>
     <t>Solo se puede escoger una dirección de las 8 posibles. Puede ser solo una casilla o todas las casillas.</t>
   </si>
+  <si>
+    <t>Rude</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2371,6 +2377,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2395,7 +2402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2414,10 +2420,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2426,59 +2432,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2507,57 +2477,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2585,9 +2504,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2595,28 +2601,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6306,7 +6312,7 @@
         <xdr:cNvPr id="2" name="AutoShape 2" descr="blob:https://web.whatsapp.com/e63e1d1b-b105-4665-8c8b-d31e2f432f37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000020C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6679,28 +6685,28 @@
       <c r="B5" s="174" t="s">
         <v>366</v>
       </c>
-      <c r="C5" s="178" t="s">
+      <c r="C5" s="183" t="s">
         <v>376</v>
       </c>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
-      <c r="G5" s="179"/>
-      <c r="H5" s="179"/>
-      <c r="I5" s="179"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="179"/>
-      <c r="L5" s="180"/>
-      <c r="M5" s="178" t="s">
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="184"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="184"/>
+      <c r="L5" s="185"/>
+      <c r="M5" s="183" t="s">
         <v>378</v>
       </c>
-      <c r="N5" s="179"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="179"/>
-      <c r="Q5" s="179"/>
-      <c r="R5" s="179"/>
-      <c r="S5" s="179"/>
-      <c r="T5" s="180"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="184"/>
+      <c r="R5" s="184"/>
+      <c r="S5" s="184"/>
+      <c r="T5" s="185"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="174"/>
@@ -6729,51 +6735,51 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="174"/>
-      <c r="C7" s="187"/>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188"/>
-      <c r="H7" s="188"/>
-      <c r="I7" s="188"/>
-      <c r="J7" s="188"/>
-      <c r="K7" s="188"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="179"/>
+      <c r="F7" s="179"/>
+      <c r="G7" s="179"/>
+      <c r="H7" s="179"/>
+      <c r="I7" s="179"/>
+      <c r="J7" s="179"/>
+      <c r="K7" s="179"/>
       <c r="L7" s="189"/>
-      <c r="M7" s="187" t="s">
+      <c r="M7" s="178" t="s">
         <v>380</v>
       </c>
-      <c r="N7" s="188"/>
-      <c r="O7" s="188"/>
-      <c r="P7" s="188"/>
-      <c r="Q7" s="188"/>
-      <c r="R7" s="188"/>
-      <c r="S7" s="188"/>
+      <c r="N7" s="179"/>
+      <c r="O7" s="179"/>
+      <c r="P7" s="179"/>
+      <c r="Q7" s="179"/>
+      <c r="R7" s="179"/>
+      <c r="S7" s="179"/>
       <c r="T7" s="189"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="174" t="s">
         <v>189</v>
       </c>
-      <c r="C8" s="178" t="s">
+      <c r="C8" s="183" t="s">
         <v>381</v>
       </c>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="179"/>
-      <c r="H8" s="179"/>
-      <c r="I8" s="179"/>
-      <c r="J8" s="179"/>
-      <c r="K8" s="179"/>
-      <c r="L8" s="180"/>
-      <c r="M8" s="178"/>
-      <c r="N8" s="179"/>
-      <c r="O8" s="179"/>
-      <c r="P8" s="179"/>
-      <c r="Q8" s="179"/>
-      <c r="R8" s="179"/>
-      <c r="S8" s="179"/>
-      <c r="T8" s="180"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="184"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="L8" s="185"/>
+      <c r="M8" s="183"/>
+      <c r="N8" s="184"/>
+      <c r="O8" s="184"/>
+      <c r="P8" s="184"/>
+      <c r="Q8" s="184"/>
+      <c r="R8" s="184"/>
+      <c r="S8" s="184"/>
+      <c r="T8" s="185"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="174"/>
@@ -6789,62 +6795,62 @@
       <c r="J9" s="176"/>
       <c r="K9" s="176"/>
       <c r="L9" s="177"/>
-      <c r="M9" s="181" t="s">
+      <c r="M9" s="186" t="s">
         <v>383</v>
       </c>
-      <c r="N9" s="182"/>
-      <c r="O9" s="182"/>
-      <c r="P9" s="182"/>
-      <c r="Q9" s="182"/>
-      <c r="R9" s="182"/>
-      <c r="S9" s="182"/>
-      <c r="T9" s="183"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="188"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="174"/>
-      <c r="C10" s="184"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
-      <c r="J10" s="185"/>
-      <c r="K10" s="185"/>
-      <c r="L10" s="186"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="188"/>
-      <c r="O10" s="188"/>
-      <c r="P10" s="188"/>
-      <c r="Q10" s="188"/>
-      <c r="R10" s="188"/>
-      <c r="S10" s="188"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="182"/>
+      <c r="M10" s="178"/>
+      <c r="N10" s="179"/>
+      <c r="O10" s="179"/>
+      <c r="P10" s="179"/>
+      <c r="Q10" s="179"/>
+      <c r="R10" s="179"/>
+      <c r="S10" s="179"/>
       <c r="T10" s="189"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="174" t="s">
         <v>364</v>
       </c>
-      <c r="C11" s="178" t="s">
+      <c r="C11" s="183" t="s">
         <v>384</v>
       </c>
-      <c r="D11" s="179"/>
-      <c r="E11" s="179"/>
-      <c r="F11" s="179"/>
-      <c r="G11" s="179"/>
-      <c r="H11" s="179"/>
-      <c r="I11" s="179"/>
-      <c r="J11" s="179"/>
-      <c r="K11" s="179"/>
-      <c r="L11" s="180"/>
-      <c r="M11" s="178"/>
-      <c r="N11" s="179"/>
-      <c r="O11" s="179"/>
-      <c r="P11" s="179"/>
-      <c r="Q11" s="179"/>
-      <c r="R11" s="179"/>
-      <c r="S11" s="179"/>
-      <c r="T11" s="180"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="184"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="184"/>
+      <c r="L11" s="185"/>
+      <c r="M11" s="183"/>
+      <c r="N11" s="184"/>
+      <c r="O11" s="184"/>
+      <c r="P11" s="184"/>
+      <c r="Q11" s="184"/>
+      <c r="R11" s="184"/>
+      <c r="S11" s="184"/>
+      <c r="T11" s="185"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="174"/>
@@ -6873,15 +6879,15 @@
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="174"/>
-      <c r="C13" s="187"/>
-      <c r="D13" s="188"/>
-      <c r="E13" s="188"/>
-      <c r="F13" s="188"/>
-      <c r="G13" s="188"/>
-      <c r="H13" s="188"/>
-      <c r="I13" s="188"/>
-      <c r="J13" s="188"/>
-      <c r="K13" s="188"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="179"/>
+      <c r="H13" s="179"/>
+      <c r="I13" s="179"/>
+      <c r="J13" s="179"/>
+      <c r="K13" s="179"/>
       <c r="L13" s="189"/>
       <c r="M13" s="175"/>
       <c r="N13" s="176"/>
@@ -6896,26 +6902,26 @@
       <c r="B14" s="174" t="s">
         <v>367</v>
       </c>
-      <c r="C14" s="178"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="179"/>
-      <c r="G14" s="179"/>
-      <c r="H14" s="179"/>
-      <c r="I14" s="179"/>
-      <c r="J14" s="179"/>
-      <c r="K14" s="179"/>
-      <c r="L14" s="179"/>
-      <c r="M14" s="178" t="s">
+      <c r="C14" s="183"/>
+      <c r="D14" s="184"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="184"/>
+      <c r="H14" s="184"/>
+      <c r="I14" s="184"/>
+      <c r="J14" s="184"/>
+      <c r="K14" s="184"/>
+      <c r="L14" s="184"/>
+      <c r="M14" s="183" t="s">
         <v>388</v>
       </c>
-      <c r="N14" s="179"/>
-      <c r="O14" s="179"/>
-      <c r="P14" s="179"/>
-      <c r="Q14" s="179"/>
-      <c r="R14" s="179"/>
-      <c r="S14" s="179"/>
-      <c r="T14" s="180"/>
+      <c r="N14" s="184"/>
+      <c r="O14" s="184"/>
+      <c r="P14" s="184"/>
+      <c r="Q14" s="184"/>
+      <c r="R14" s="184"/>
+      <c r="S14" s="184"/>
+      <c r="T14" s="185"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="174"/>
@@ -6944,24 +6950,24 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="174"/>
-      <c r="C16" s="187"/>
-      <c r="D16" s="188"/>
-      <c r="E16" s="188"/>
-      <c r="F16" s="188"/>
-      <c r="G16" s="188"/>
-      <c r="H16" s="188"/>
-      <c r="I16" s="188"/>
-      <c r="J16" s="188"/>
-      <c r="K16" s="188"/>
-      <c r="L16" s="188"/>
-      <c r="M16" s="184"/>
-      <c r="N16" s="185"/>
-      <c r="O16" s="185"/>
-      <c r="P16" s="185"/>
-      <c r="Q16" s="185"/>
-      <c r="R16" s="185"/>
-      <c r="S16" s="185"/>
-      <c r="T16" s="186"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="179"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="179"/>
+      <c r="J16" s="179"/>
+      <c r="K16" s="179"/>
+      <c r="L16" s="179"/>
+      <c r="M16" s="180"/>
+      <c r="N16" s="181"/>
+      <c r="O16" s="181"/>
+      <c r="P16" s="181"/>
+      <c r="Q16" s="181"/>
+      <c r="R16" s="181"/>
+      <c r="S16" s="181"/>
+      <c r="T16" s="182"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="70"/>
@@ -6978,18 +6984,18 @@
       <c r="B21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="192" t="s">
+      <c r="C21" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="192"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
-      <c r="K21" s="192"/>
-      <c r="L21" s="192"/>
+      <c r="D21" s="193"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="193"/>
+      <c r="L21" s="193"/>
       <c r="M21" s="191" t="s">
         <v>96</v>
       </c>
@@ -7002,32 +7008,32 @@
       <c r="T21" s="191"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="190" t="s">
+      <c r="B22" s="192" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="178" t="s">
+      <c r="C22" s="183" t="s">
         <v>394</v>
       </c>
-      <c r="D22" s="179"/>
-      <c r="E22" s="179"/>
-      <c r="F22" s="179"/>
-      <c r="G22" s="179"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="179"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="180"/>
-      <c r="M22" s="179"/>
-      <c r="N22" s="179"/>
-      <c r="O22" s="179"/>
-      <c r="P22" s="179"/>
-      <c r="Q22" s="179"/>
-      <c r="R22" s="179"/>
-      <c r="S22" s="179"/>
-      <c r="T22" s="180"/>
+      <c r="D22" s="184"/>
+      <c r="E22" s="184"/>
+      <c r="F22" s="184"/>
+      <c r="G22" s="184"/>
+      <c r="H22" s="184"/>
+      <c r="I22" s="184"/>
+      <c r="J22" s="184"/>
+      <c r="K22" s="184"/>
+      <c r="L22" s="185"/>
+      <c r="M22" s="184"/>
+      <c r="N22" s="184"/>
+      <c r="O22" s="184"/>
+      <c r="P22" s="184"/>
+      <c r="Q22" s="184"/>
+      <c r="R22" s="184"/>
+      <c r="S22" s="184"/>
+      <c r="T22" s="185"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="190"/>
+      <c r="B23" s="192"/>
       <c r="C23" s="175" t="s">
         <v>395</v>
       </c>
@@ -7052,24 +7058,24 @@
       <c r="T23" s="177"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="190"/>
-      <c r="C24" s="184"/>
-      <c r="D24" s="185"/>
-      <c r="E24" s="185"/>
-      <c r="F24" s="185"/>
-      <c r="G24" s="185"/>
-      <c r="H24" s="185"/>
-      <c r="I24" s="185"/>
-      <c r="J24" s="185"/>
-      <c r="K24" s="185"/>
-      <c r="L24" s="186"/>
-      <c r="M24" s="188"/>
-      <c r="N24" s="188"/>
-      <c r="O24" s="188"/>
-      <c r="P24" s="188"/>
-      <c r="Q24" s="188"/>
-      <c r="R24" s="188"/>
-      <c r="S24" s="188"/>
+      <c r="B24" s="192"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="181"/>
+      <c r="L24" s="182"/>
+      <c r="M24" s="179"/>
+      <c r="N24" s="179"/>
+      <c r="O24" s="179"/>
+      <c r="P24" s="179"/>
+      <c r="Q24" s="179"/>
+      <c r="R24" s="179"/>
+      <c r="S24" s="179"/>
       <c r="T24" s="189"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -7086,14 +7092,14 @@
       <c r="J25" s="176"/>
       <c r="K25" s="176"/>
       <c r="L25" s="177"/>
-      <c r="M25" s="178"/>
-      <c r="N25" s="179"/>
-      <c r="O25" s="179"/>
-      <c r="P25" s="179"/>
-      <c r="Q25" s="179"/>
-      <c r="R25" s="179"/>
-      <c r="S25" s="179"/>
-      <c r="T25" s="180"/>
+      <c r="M25" s="183"/>
+      <c r="N25" s="184"/>
+      <c r="O25" s="184"/>
+      <c r="P25" s="184"/>
+      <c r="Q25" s="184"/>
+      <c r="R25" s="184"/>
+      <c r="S25" s="184"/>
+      <c r="T25" s="185"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="174"/>
@@ -7109,67 +7115,67 @@
       <c r="J26" s="176"/>
       <c r="K26" s="176"/>
       <c r="L26" s="177"/>
-      <c r="M26" s="181" t="s">
+      <c r="M26" s="186" t="s">
         <v>442</v>
       </c>
-      <c r="N26" s="182"/>
-      <c r="O26" s="182"/>
-      <c r="P26" s="182"/>
-      <c r="Q26" s="182"/>
-      <c r="R26" s="182"/>
-      <c r="S26" s="182"/>
-      <c r="T26" s="183"/>
+      <c r="N26" s="187"/>
+      <c r="O26" s="187"/>
+      <c r="P26" s="187"/>
+      <c r="Q26" s="187"/>
+      <c r="R26" s="187"/>
+      <c r="S26" s="187"/>
+      <c r="T26" s="188"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="174"/>
-      <c r="C27" s="184"/>
-      <c r="D27" s="185"/>
-      <c r="E27" s="185"/>
-      <c r="F27" s="185"/>
-      <c r="G27" s="185"/>
-      <c r="H27" s="185"/>
-      <c r="I27" s="185"/>
-      <c r="J27" s="185"/>
-      <c r="K27" s="185"/>
-      <c r="L27" s="186"/>
-      <c r="M27" s="187"/>
-      <c r="N27" s="188"/>
-      <c r="O27" s="188"/>
-      <c r="P27" s="188"/>
-      <c r="Q27" s="188"/>
-      <c r="R27" s="188"/>
-      <c r="S27" s="188"/>
+      <c r="C27" s="180"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="181"/>
+      <c r="J27" s="181"/>
+      <c r="K27" s="181"/>
+      <c r="L27" s="182"/>
+      <c r="M27" s="178"/>
+      <c r="N27" s="179"/>
+      <c r="O27" s="179"/>
+      <c r="P27" s="179"/>
+      <c r="Q27" s="179"/>
+      <c r="R27" s="179"/>
+      <c r="S27" s="179"/>
       <c r="T27" s="189"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="190" t="s">
+      <c r="B28" s="192" t="s">
         <v>365</v>
       </c>
-      <c r="C28" s="178" t="s">
+      <c r="C28" s="183" t="s">
         <v>398</v>
       </c>
-      <c r="D28" s="179"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="179"/>
-      <c r="L28" s="180"/>
-      <c r="M28" s="179" t="s">
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="184"/>
+      <c r="I28" s="184"/>
+      <c r="J28" s="184"/>
+      <c r="K28" s="184"/>
+      <c r="L28" s="185"/>
+      <c r="M28" s="184" t="s">
         <v>400</v>
       </c>
-      <c r="N28" s="179"/>
-      <c r="O28" s="179"/>
-      <c r="P28" s="179"/>
-      <c r="Q28" s="179"/>
-      <c r="R28" s="179"/>
-      <c r="S28" s="179"/>
-      <c r="T28" s="180"/>
+      <c r="N28" s="184"/>
+      <c r="O28" s="184"/>
+      <c r="P28" s="184"/>
+      <c r="Q28" s="184"/>
+      <c r="R28" s="184"/>
+      <c r="S28" s="184"/>
+      <c r="T28" s="185"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="190"/>
+      <c r="B29" s="192"/>
       <c r="C29" s="175" t="s">
         <v>399</v>
       </c>
@@ -7194,17 +7200,17 @@
       <c r="T29" s="177"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="190"/>
-      <c r="C30" s="184"/>
-      <c r="D30" s="185"/>
-      <c r="E30" s="185"/>
-      <c r="F30" s="185"/>
-      <c r="G30" s="185"/>
-      <c r="H30" s="185"/>
-      <c r="I30" s="185"/>
-      <c r="J30" s="185"/>
-      <c r="K30" s="185"/>
-      <c r="L30" s="186"/>
+      <c r="B30" s="192"/>
+      <c r="C30" s="180"/>
+      <c r="D30" s="181"/>
+      <c r="E30" s="181"/>
+      <c r="F30" s="181"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="181"/>
+      <c r="I30" s="181"/>
+      <c r="J30" s="181"/>
+      <c r="K30" s="181"/>
+      <c r="L30" s="182"/>
       <c r="M30" s="176"/>
       <c r="N30" s="176"/>
       <c r="O30" s="176"/>
@@ -7228,16 +7234,16 @@
       <c r="J31" s="176"/>
       <c r="K31" s="176"/>
       <c r="L31" s="176"/>
-      <c r="M31" s="178" t="s">
+      <c r="M31" s="183" t="s">
         <v>403</v>
       </c>
-      <c r="N31" s="179"/>
-      <c r="O31" s="179"/>
-      <c r="P31" s="179"/>
-      <c r="Q31" s="179"/>
-      <c r="R31" s="179"/>
-      <c r="S31" s="179"/>
-      <c r="T31" s="180"/>
+      <c r="N31" s="184"/>
+      <c r="O31" s="184"/>
+      <c r="P31" s="184"/>
+      <c r="Q31" s="184"/>
+      <c r="R31" s="184"/>
+      <c r="S31" s="184"/>
+      <c r="T31" s="185"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="174"/>
@@ -7253,37 +7259,37 @@
       <c r="J32" s="176"/>
       <c r="K32" s="176"/>
       <c r="L32" s="176"/>
-      <c r="M32" s="181" t="s">
+      <c r="M32" s="186" t="s">
         <v>441</v>
       </c>
-      <c r="N32" s="182"/>
-      <c r="O32" s="182"/>
-      <c r="P32" s="182"/>
-      <c r="Q32" s="182"/>
-      <c r="R32" s="182"/>
-      <c r="S32" s="182"/>
-      <c r="T32" s="183"/>
+      <c r="N32" s="187"/>
+      <c r="O32" s="187"/>
+      <c r="P32" s="187"/>
+      <c r="Q32" s="187"/>
+      <c r="R32" s="187"/>
+      <c r="S32" s="187"/>
+      <c r="T32" s="188"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="174"/>
-      <c r="C33" s="187"/>
-      <c r="D33" s="188"/>
-      <c r="E33" s="188"/>
-      <c r="F33" s="188"/>
-      <c r="G33" s="188"/>
-      <c r="H33" s="188"/>
-      <c r="I33" s="188"/>
-      <c r="J33" s="188"/>
-      <c r="K33" s="188"/>
-      <c r="L33" s="188"/>
-      <c r="M33" s="184"/>
-      <c r="N33" s="185"/>
-      <c r="O33" s="185"/>
-      <c r="P33" s="185"/>
-      <c r="Q33" s="185"/>
-      <c r="R33" s="185"/>
-      <c r="S33" s="185"/>
-      <c r="T33" s="186"/>
+      <c r="C33" s="178"/>
+      <c r="D33" s="179"/>
+      <c r="E33" s="179"/>
+      <c r="F33" s="179"/>
+      <c r="G33" s="179"/>
+      <c r="H33" s="179"/>
+      <c r="I33" s="179"/>
+      <c r="J33" s="179"/>
+      <c r="K33" s="179"/>
+      <c r="L33" s="179"/>
+      <c r="M33" s="180"/>
+      <c r="N33" s="181"/>
+      <c r="O33" s="181"/>
+      <c r="P33" s="181"/>
+      <c r="Q33" s="181"/>
+      <c r="R33" s="181"/>
+      <c r="S33" s="181"/>
+      <c r="T33" s="182"/>
     </row>
     <row r="36" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
@@ -7321,43 +7327,43 @@
       <c r="B39" s="174" t="s">
         <v>370</v>
       </c>
-      <c r="C39" s="178" t="s">
+      <c r="C39" s="183" t="s">
         <v>404</v>
       </c>
-      <c r="D39" s="179"/>
-      <c r="E39" s="179"/>
-      <c r="F39" s="179"/>
-      <c r="G39" s="179"/>
-      <c r="H39" s="179"/>
-      <c r="I39" s="179"/>
-      <c r="J39" s="179"/>
-      <c r="K39" s="179"/>
-      <c r="L39" s="180"/>
-      <c r="M39" s="178" t="s">
+      <c r="D39" s="184"/>
+      <c r="E39" s="184"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="184"/>
+      <c r="I39" s="184"/>
+      <c r="J39" s="184"/>
+      <c r="K39" s="184"/>
+      <c r="L39" s="185"/>
+      <c r="M39" s="183" t="s">
         <v>405</v>
       </c>
-      <c r="N39" s="179"/>
-      <c r="O39" s="179"/>
-      <c r="P39" s="179"/>
-      <c r="Q39" s="179"/>
-      <c r="R39" s="179"/>
-      <c r="S39" s="179"/>
-      <c r="T39" s="180"/>
+      <c r="N39" s="184"/>
+      <c r="O39" s="184"/>
+      <c r="P39" s="184"/>
+      <c r="Q39" s="184"/>
+      <c r="R39" s="184"/>
+      <c r="S39" s="184"/>
+      <c r="T39" s="185"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="174"/>
-      <c r="C40" s="181" t="s">
+      <c r="C40" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D40" s="193"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="193"/>
-      <c r="G40" s="193"/>
-      <c r="H40" s="193"/>
-      <c r="I40" s="193"/>
-      <c r="J40" s="193"/>
-      <c r="K40" s="193"/>
-      <c r="L40" s="183"/>
+      <c r="D40" s="190"/>
+      <c r="E40" s="190"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="190"/>
+      <c r="H40" s="190"/>
+      <c r="I40" s="190"/>
+      <c r="J40" s="190"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="188"/>
       <c r="M40" s="175" t="s">
         <v>406</v>
       </c>
@@ -7371,143 +7377,143 @@
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="174"/>
-      <c r="C41" s="187" t="s">
+      <c r="C41" s="178" t="s">
         <v>419</v>
       </c>
-      <c r="D41" s="188"/>
-      <c r="E41" s="188"/>
-      <c r="F41" s="188"/>
-      <c r="G41" s="188"/>
-      <c r="H41" s="188"/>
-      <c r="I41" s="188"/>
-      <c r="J41" s="188"/>
-      <c r="K41" s="188"/>
+      <c r="D41" s="179"/>
+      <c r="E41" s="179"/>
+      <c r="F41" s="179"/>
+      <c r="G41" s="179"/>
+      <c r="H41" s="179"/>
+      <c r="I41" s="179"/>
+      <c r="J41" s="179"/>
+      <c r="K41" s="179"/>
       <c r="L41" s="189"/>
-      <c r="M41" s="187"/>
-      <c r="N41" s="188"/>
-      <c r="O41" s="188"/>
-      <c r="P41" s="188"/>
-      <c r="Q41" s="188"/>
-      <c r="R41" s="188"/>
-      <c r="S41" s="188"/>
+      <c r="M41" s="178"/>
+      <c r="N41" s="179"/>
+      <c r="O41" s="179"/>
+      <c r="P41" s="179"/>
+      <c r="Q41" s="179"/>
+      <c r="R41" s="179"/>
+      <c r="S41" s="179"/>
       <c r="T41" s="189"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="174" t="s">
         <v>371</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="183" t="s">
         <v>407</v>
       </c>
-      <c r="D42" s="179"/>
-      <c r="E42" s="179"/>
-      <c r="F42" s="179"/>
-      <c r="G42" s="179"/>
-      <c r="H42" s="179"/>
-      <c r="I42" s="179"/>
-      <c r="J42" s="179"/>
-      <c r="K42" s="179"/>
-      <c r="L42" s="180"/>
-      <c r="M42" s="178"/>
-      <c r="N42" s="179"/>
-      <c r="O42" s="179"/>
-      <c r="P42" s="179"/>
-      <c r="Q42" s="179"/>
-      <c r="R42" s="179"/>
-      <c r="S42" s="179"/>
-      <c r="T42" s="180"/>
+      <c r="D42" s="184"/>
+      <c r="E42" s="184"/>
+      <c r="F42" s="184"/>
+      <c r="G42" s="184"/>
+      <c r="H42" s="184"/>
+      <c r="I42" s="184"/>
+      <c r="J42" s="184"/>
+      <c r="K42" s="184"/>
+      <c r="L42" s="185"/>
+      <c r="M42" s="183"/>
+      <c r="N42" s="184"/>
+      <c r="O42" s="184"/>
+      <c r="P42" s="184"/>
+      <c r="Q42" s="184"/>
+      <c r="R42" s="184"/>
+      <c r="S42" s="184"/>
+      <c r="T42" s="185"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="174"/>
-      <c r="C43" s="181" t="s">
+      <c r="C43" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D43" s="193"/>
-      <c r="E43" s="193"/>
-      <c r="F43" s="193"/>
-      <c r="G43" s="193"/>
-      <c r="H43" s="193"/>
-      <c r="I43" s="193"/>
-      <c r="J43" s="193"/>
-      <c r="K43" s="193"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="181" t="s">
+      <c r="D43" s="190"/>
+      <c r="E43" s="190"/>
+      <c r="F43" s="190"/>
+      <c r="G43" s="190"/>
+      <c r="H43" s="190"/>
+      <c r="I43" s="190"/>
+      <c r="J43" s="190"/>
+      <c r="K43" s="190"/>
+      <c r="L43" s="188"/>
+      <c r="M43" s="186" t="s">
         <v>438</v>
       </c>
-      <c r="N43" s="182"/>
-      <c r="O43" s="182"/>
-      <c r="P43" s="182"/>
-      <c r="Q43" s="182"/>
-      <c r="R43" s="182"/>
-      <c r="S43" s="182"/>
-      <c r="T43" s="183"/>
+      <c r="N43" s="187"/>
+      <c r="O43" s="187"/>
+      <c r="P43" s="187"/>
+      <c r="Q43" s="187"/>
+      <c r="R43" s="187"/>
+      <c r="S43" s="187"/>
+      <c r="T43" s="188"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="174"/>
-      <c r="C44" s="184" t="s">
+      <c r="C44" s="180" t="s">
         <v>423</v>
       </c>
-      <c r="D44" s="185"/>
-      <c r="E44" s="185"/>
-      <c r="F44" s="185"/>
-      <c r="G44" s="185"/>
-      <c r="H44" s="185"/>
-      <c r="I44" s="185"/>
-      <c r="J44" s="185"/>
-      <c r="K44" s="185"/>
-      <c r="L44" s="186"/>
-      <c r="M44" s="187" t="s">
+      <c r="D44" s="181"/>
+      <c r="E44" s="181"/>
+      <c r="F44" s="181"/>
+      <c r="G44" s="181"/>
+      <c r="H44" s="181"/>
+      <c r="I44" s="181"/>
+      <c r="J44" s="181"/>
+      <c r="K44" s="181"/>
+      <c r="L44" s="182"/>
+      <c r="M44" s="178" t="s">
         <v>408</v>
       </c>
-      <c r="N44" s="188"/>
-      <c r="O44" s="188"/>
-      <c r="P44" s="188"/>
-      <c r="Q44" s="188"/>
-      <c r="R44" s="188"/>
-      <c r="S44" s="188"/>
+      <c r="N44" s="179"/>
+      <c r="O44" s="179"/>
+      <c r="P44" s="179"/>
+      <c r="Q44" s="179"/>
+      <c r="R44" s="179"/>
+      <c r="S44" s="179"/>
       <c r="T44" s="189"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="174" t="s">
         <v>392</v>
       </c>
-      <c r="C45" s="178" t="s">
+      <c r="C45" s="183" t="s">
         <v>411</v>
       </c>
-      <c r="D45" s="179"/>
-      <c r="E45" s="179"/>
-      <c r="F45" s="179"/>
-      <c r="G45" s="179"/>
-      <c r="H45" s="179"/>
-      <c r="I45" s="179"/>
-      <c r="J45" s="179"/>
-      <c r="K45" s="179"/>
-      <c r="L45" s="180"/>
-      <c r="M45" s="178" t="s">
+      <c r="D45" s="184"/>
+      <c r="E45" s="184"/>
+      <c r="F45" s="184"/>
+      <c r="G45" s="184"/>
+      <c r="H45" s="184"/>
+      <c r="I45" s="184"/>
+      <c r="J45" s="184"/>
+      <c r="K45" s="184"/>
+      <c r="L45" s="185"/>
+      <c r="M45" s="183" t="s">
         <v>439</v>
       </c>
-      <c r="N45" s="179"/>
-      <c r="O45" s="179"/>
-      <c r="P45" s="179"/>
-      <c r="Q45" s="179"/>
-      <c r="R45" s="179"/>
-      <c r="S45" s="179"/>
-      <c r="T45" s="180"/>
+      <c r="N45" s="184"/>
+      <c r="O45" s="184"/>
+      <c r="P45" s="184"/>
+      <c r="Q45" s="184"/>
+      <c r="R45" s="184"/>
+      <c r="S45" s="184"/>
+      <c r="T45" s="185"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="174"/>
-      <c r="C46" s="181" t="s">
+      <c r="C46" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D46" s="193"/>
-      <c r="E46" s="193"/>
-      <c r="F46" s="193"/>
-      <c r="G46" s="193"/>
-      <c r="H46" s="193"/>
-      <c r="I46" s="193"/>
-      <c r="J46" s="193"/>
-      <c r="K46" s="193"/>
-      <c r="L46" s="183"/>
+      <c r="D46" s="190"/>
+      <c r="E46" s="190"/>
+      <c r="F46" s="190"/>
+      <c r="G46" s="190"/>
+      <c r="H46" s="190"/>
+      <c r="I46" s="190"/>
+      <c r="J46" s="190"/>
+      <c r="K46" s="190"/>
+      <c r="L46" s="188"/>
       <c r="M46" s="175" t="s">
         <v>409</v>
       </c>
@@ -7521,70 +7527,70 @@
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="174"/>
-      <c r="C47" s="187" t="s">
+      <c r="C47" s="178" t="s">
         <v>421</v>
       </c>
-      <c r="D47" s="188"/>
-      <c r="E47" s="188"/>
-      <c r="F47" s="188"/>
-      <c r="G47" s="188"/>
-      <c r="H47" s="188"/>
-      <c r="I47" s="188"/>
-      <c r="J47" s="188"/>
-      <c r="K47" s="188"/>
+      <c r="D47" s="179"/>
+      <c r="E47" s="179"/>
+      <c r="F47" s="179"/>
+      <c r="G47" s="179"/>
+      <c r="H47" s="179"/>
+      <c r="I47" s="179"/>
+      <c r="J47" s="179"/>
+      <c r="K47" s="179"/>
       <c r="L47" s="189"/>
-      <c r="M47" s="184" t="s">
+      <c r="M47" s="180" t="s">
         <v>410</v>
       </c>
-      <c r="N47" s="185"/>
-      <c r="O47" s="185"/>
-      <c r="P47" s="185"/>
-      <c r="Q47" s="185"/>
-      <c r="R47" s="185"/>
-      <c r="S47" s="185"/>
-      <c r="T47" s="186"/>
+      <c r="N47" s="181"/>
+      <c r="O47" s="181"/>
+      <c r="P47" s="181"/>
+      <c r="Q47" s="181"/>
+      <c r="R47" s="181"/>
+      <c r="S47" s="181"/>
+      <c r="T47" s="182"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="174" t="s">
         <v>368</v>
       </c>
-      <c r="C48" s="178" t="s">
+      <c r="C48" s="183" t="s">
         <v>412</v>
       </c>
-      <c r="D48" s="179"/>
-      <c r="E48" s="179"/>
-      <c r="F48" s="179"/>
-      <c r="G48" s="179"/>
-      <c r="H48" s="179"/>
-      <c r="I48" s="179"/>
-      <c r="J48" s="179"/>
-      <c r="K48" s="179"/>
-      <c r="L48" s="180"/>
-      <c r="M48" s="178" t="s">
+      <c r="D48" s="184"/>
+      <c r="E48" s="184"/>
+      <c r="F48" s="184"/>
+      <c r="G48" s="184"/>
+      <c r="H48" s="184"/>
+      <c r="I48" s="184"/>
+      <c r="J48" s="184"/>
+      <c r="K48" s="184"/>
+      <c r="L48" s="185"/>
+      <c r="M48" s="183" t="s">
         <v>440</v>
       </c>
-      <c r="N48" s="179"/>
-      <c r="O48" s="179"/>
-      <c r="P48" s="179"/>
-      <c r="Q48" s="179"/>
-      <c r="R48" s="179"/>
-      <c r="S48" s="179"/>
-      <c r="T48" s="180"/>
+      <c r="N48" s="184"/>
+      <c r="O48" s="184"/>
+      <c r="P48" s="184"/>
+      <c r="Q48" s="184"/>
+      <c r="R48" s="184"/>
+      <c r="S48" s="184"/>
+      <c r="T48" s="185"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" s="174"/>
-      <c r="C49" s="181" t="s">
+      <c r="C49" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D49" s="193"/>
-      <c r="E49" s="193"/>
-      <c r="F49" s="193"/>
-      <c r="G49" s="193"/>
-      <c r="H49" s="193"/>
-      <c r="I49" s="193"/>
-      <c r="J49" s="193"/>
-      <c r="K49" s="193"/>
-      <c r="L49" s="183"/>
+      <c r="D49" s="190"/>
+      <c r="E49" s="190"/>
+      <c r="F49" s="190"/>
+      <c r="G49" s="190"/>
+      <c r="H49" s="190"/>
+      <c r="I49" s="190"/>
+      <c r="J49" s="190"/>
+      <c r="K49" s="190"/>
+      <c r="L49" s="188"/>
       <c r="M49" s="175" t="s">
         <v>413</v>
       </c>
@@ -7598,103 +7604,103 @@
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" s="174"/>
-      <c r="C50" s="187" t="s">
+      <c r="C50" s="178" t="s">
         <v>422</v>
       </c>
-      <c r="D50" s="188"/>
-      <c r="E50" s="188"/>
-      <c r="F50" s="188"/>
-      <c r="G50" s="188"/>
-      <c r="H50" s="188"/>
-      <c r="I50" s="188"/>
-      <c r="J50" s="188"/>
-      <c r="K50" s="188"/>
+      <c r="D50" s="179"/>
+      <c r="E50" s="179"/>
+      <c r="F50" s="179"/>
+      <c r="G50" s="179"/>
+      <c r="H50" s="179"/>
+      <c r="I50" s="179"/>
+      <c r="J50" s="179"/>
+      <c r="K50" s="179"/>
       <c r="L50" s="189"/>
-      <c r="M50" s="181" t="s">
+      <c r="M50" s="186" t="s">
         <v>414</v>
       </c>
-      <c r="N50" s="182"/>
-      <c r="O50" s="182"/>
-      <c r="P50" s="182"/>
-      <c r="Q50" s="182"/>
-      <c r="R50" s="182"/>
-      <c r="S50" s="182"/>
-      <c r="T50" s="183"/>
+      <c r="N50" s="187"/>
+      <c r="O50" s="187"/>
+      <c r="P50" s="187"/>
+      <c r="Q50" s="187"/>
+      <c r="R50" s="187"/>
+      <c r="S50" s="187"/>
+      <c r="T50" s="188"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51" s="174" t="s">
         <v>369</v>
       </c>
-      <c r="C51" s="178" t="s">
+      <c r="C51" s="183" t="s">
         <v>417</v>
       </c>
-      <c r="D51" s="179"/>
-      <c r="E51" s="179"/>
-      <c r="F51" s="179"/>
-      <c r="G51" s="179"/>
-      <c r="H51" s="179"/>
-      <c r="I51" s="179"/>
-      <c r="J51" s="179"/>
-      <c r="K51" s="179"/>
-      <c r="L51" s="180"/>
-      <c r="M51" s="178" t="s">
+      <c r="D51" s="184"/>
+      <c r="E51" s="184"/>
+      <c r="F51" s="184"/>
+      <c r="G51" s="184"/>
+      <c r="H51" s="184"/>
+      <c r="I51" s="184"/>
+      <c r="J51" s="184"/>
+      <c r="K51" s="184"/>
+      <c r="L51" s="185"/>
+      <c r="M51" s="183" t="s">
         <v>415</v>
       </c>
-      <c r="N51" s="179"/>
-      <c r="O51" s="179"/>
-      <c r="P51" s="179"/>
-      <c r="Q51" s="179"/>
-      <c r="R51" s="179"/>
-      <c r="S51" s="179"/>
-      <c r="T51" s="180"/>
+      <c r="N51" s="184"/>
+      <c r="O51" s="184"/>
+      <c r="P51" s="184"/>
+      <c r="Q51" s="184"/>
+      <c r="R51" s="184"/>
+      <c r="S51" s="184"/>
+      <c r="T51" s="185"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52" s="174"/>
-      <c r="C52" s="181" t="s">
+      <c r="C52" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D52" s="193"/>
-      <c r="E52" s="193"/>
-      <c r="F52" s="193"/>
-      <c r="G52" s="193"/>
-      <c r="H52" s="193"/>
-      <c r="I52" s="193"/>
-      <c r="J52" s="193"/>
-      <c r="K52" s="193"/>
-      <c r="L52" s="183"/>
-      <c r="M52" s="181" t="s">
+      <c r="D52" s="190"/>
+      <c r="E52" s="190"/>
+      <c r="F52" s="190"/>
+      <c r="G52" s="190"/>
+      <c r="H52" s="190"/>
+      <c r="I52" s="190"/>
+      <c r="J52" s="190"/>
+      <c r="K52" s="190"/>
+      <c r="L52" s="188"/>
+      <c r="M52" s="186" t="s">
         <v>416</v>
       </c>
-      <c r="N52" s="182"/>
-      <c r="O52" s="182"/>
-      <c r="P52" s="182"/>
-      <c r="Q52" s="182"/>
-      <c r="R52" s="182"/>
-      <c r="S52" s="182"/>
-      <c r="T52" s="183"/>
+      <c r="N52" s="187"/>
+      <c r="O52" s="187"/>
+      <c r="P52" s="187"/>
+      <c r="Q52" s="187"/>
+      <c r="R52" s="187"/>
+      <c r="S52" s="187"/>
+      <c r="T52" s="188"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" s="174"/>
-      <c r="C53" s="187" t="s">
+      <c r="C53" s="178" t="s">
         <v>420</v>
       </c>
-      <c r="D53" s="188"/>
-      <c r="E53" s="188"/>
-      <c r="F53" s="188"/>
-      <c r="G53" s="188"/>
-      <c r="H53" s="188"/>
-      <c r="I53" s="188"/>
-      <c r="J53" s="188"/>
-      <c r="K53" s="188"/>
+      <c r="D53" s="179"/>
+      <c r="E53" s="179"/>
+      <c r="F53" s="179"/>
+      <c r="G53" s="179"/>
+      <c r="H53" s="179"/>
+      <c r="I53" s="179"/>
+      <c r="J53" s="179"/>
+      <c r="K53" s="179"/>
       <c r="L53" s="189"/>
-      <c r="M53" s="184"/>
-      <c r="N53" s="185"/>
-      <c r="O53" s="185"/>
-      <c r="P53" s="185"/>
-      <c r="Q53" s="185"/>
-      <c r="R53" s="185"/>
-      <c r="S53" s="185"/>
-      <c r="T53" s="186"/>
+      <c r="M53" s="180"/>
+      <c r="N53" s="181"/>
+      <c r="O53" s="181"/>
+      <c r="P53" s="181"/>
+      <c r="Q53" s="181"/>
+      <c r="R53" s="181"/>
+      <c r="S53" s="181"/>
+      <c r="T53" s="182"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54" s="174" t="s">
@@ -7723,18 +7729,18 @@
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="174"/>
-      <c r="C55" s="181" t="s">
+      <c r="C55" s="186" t="s">
         <v>425</v>
       </c>
-      <c r="D55" s="193"/>
-      <c r="E55" s="193"/>
-      <c r="F55" s="193"/>
-      <c r="G55" s="193"/>
-      <c r="H55" s="193"/>
-      <c r="I55" s="193"/>
-      <c r="J55" s="193"/>
-      <c r="K55" s="193"/>
-      <c r="L55" s="183"/>
+      <c r="D55" s="190"/>
+      <c r="E55" s="190"/>
+      <c r="F55" s="190"/>
+      <c r="G55" s="190"/>
+      <c r="H55" s="190"/>
+      <c r="I55" s="190"/>
+      <c r="J55" s="190"/>
+      <c r="K55" s="190"/>
+      <c r="L55" s="188"/>
       <c r="M55" s="175" t="s">
         <v>418</v>
       </c>
@@ -7748,95 +7754,43 @@
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" s="174"/>
-      <c r="C56" s="187" t="s">
+      <c r="C56" s="178" t="s">
         <v>424</v>
       </c>
-      <c r="D56" s="188"/>
-      <c r="E56" s="188"/>
-      <c r="F56" s="188"/>
-      <c r="G56" s="188"/>
-      <c r="H56" s="188"/>
-      <c r="I56" s="188"/>
-      <c r="J56" s="188"/>
-      <c r="K56" s="188"/>
-      <c r="L56" s="188"/>
-      <c r="M56" s="184"/>
-      <c r="N56" s="185"/>
-      <c r="O56" s="185"/>
-      <c r="P56" s="185"/>
-      <c r="Q56" s="185"/>
-      <c r="R56" s="185"/>
-      <c r="S56" s="185"/>
-      <c r="T56" s="186"/>
+      <c r="D56" s="179"/>
+      <c r="E56" s="179"/>
+      <c r="F56" s="179"/>
+      <c r="G56" s="179"/>
+      <c r="H56" s="179"/>
+      <c r="I56" s="179"/>
+      <c r="J56" s="179"/>
+      <c r="K56" s="179"/>
+      <c r="L56" s="179"/>
+      <c r="M56" s="180"/>
+      <c r="N56" s="181"/>
+      <c r="O56" s="181"/>
+      <c r="P56" s="181"/>
+      <c r="Q56" s="181"/>
+      <c r="R56" s="181"/>
+      <c r="S56" s="181"/>
+      <c r="T56" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="M54:T54"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="M55:T55"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="M56:T56"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:L51"/>
-    <mergeCell ref="M51:T51"/>
-    <mergeCell ref="M52:T52"/>
-    <mergeCell ref="C53:L53"/>
-    <mergeCell ref="M53:T53"/>
-    <mergeCell ref="C52:L52"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="M48:T48"/>
-    <mergeCell ref="M49:T49"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="M50:T50"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="M45:T45"/>
-    <mergeCell ref="M46:T46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="M47:T47"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C49:L49"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:L31"/>
-    <mergeCell ref="C32:L32"/>
-    <mergeCell ref="M31:T31"/>
-    <mergeCell ref="C33:L33"/>
-    <mergeCell ref="M33:T33"/>
-    <mergeCell ref="M32:T32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:L42"/>
-    <mergeCell ref="M42:T42"/>
-    <mergeCell ref="M43:T43"/>
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="M44:T44"/>
-    <mergeCell ref="C38:L38"/>
-    <mergeCell ref="M38:T38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:L39"/>
-    <mergeCell ref="M39:T39"/>
-    <mergeCell ref="M40:T40"/>
-    <mergeCell ref="C41:L41"/>
-    <mergeCell ref="M41:T41"/>
-    <mergeCell ref="C40:L40"/>
-    <mergeCell ref="C43:L43"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:L22"/>
-    <mergeCell ref="M22:T22"/>
-    <mergeCell ref="C23:L23"/>
-    <mergeCell ref="M23:T23"/>
-    <mergeCell ref="M24:T24"/>
-    <mergeCell ref="C24:L24"/>
-    <mergeCell ref="M6:T6"/>
-    <mergeCell ref="M7:T7"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="M9:T9"/>
-    <mergeCell ref="M10:T10"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="M21:T21"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:L25"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="M27:T27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="M28:T28"/>
+    <mergeCell ref="C30:L30"/>
+    <mergeCell ref="M29:T29"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="M30:T30"/>
     <mergeCell ref="M4:T4"/>
     <mergeCell ref="C5:L5"/>
     <mergeCell ref="C6:L6"/>
@@ -7861,20 +7815,72 @@
     <mergeCell ref="M13:T13"/>
     <mergeCell ref="M14:T14"/>
     <mergeCell ref="M15:T15"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:L25"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="C26:L26"/>
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="M27:T27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="M28:T28"/>
-    <mergeCell ref="C30:L30"/>
-    <mergeCell ref="M29:T29"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="M30:T30"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:L22"/>
+    <mergeCell ref="M22:T22"/>
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="M23:T23"/>
+    <mergeCell ref="M24:T24"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="M6:T6"/>
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="M9:T9"/>
+    <mergeCell ref="M10:T10"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="C21:L21"/>
+    <mergeCell ref="M21:T21"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:L31"/>
+    <mergeCell ref="C32:L32"/>
+    <mergeCell ref="M31:T31"/>
+    <mergeCell ref="C33:L33"/>
+    <mergeCell ref="M33:T33"/>
+    <mergeCell ref="M32:T32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:L42"/>
+    <mergeCell ref="M42:T42"/>
+    <mergeCell ref="M43:T43"/>
+    <mergeCell ref="C44:L44"/>
+    <mergeCell ref="M44:T44"/>
+    <mergeCell ref="C38:L38"/>
+    <mergeCell ref="M38:T38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:L39"/>
+    <mergeCell ref="M39:T39"/>
+    <mergeCell ref="M40:T40"/>
+    <mergeCell ref="C41:L41"/>
+    <mergeCell ref="M41:T41"/>
+    <mergeCell ref="C40:L40"/>
+    <mergeCell ref="C43:L43"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="M48:T48"/>
+    <mergeCell ref="M49:T49"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="M50:T50"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="M45:T45"/>
+    <mergeCell ref="M46:T46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="M47:T47"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C49:L49"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="M54:T54"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="M55:T55"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="M56:T56"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:L51"/>
+    <mergeCell ref="M51:T51"/>
+    <mergeCell ref="M52:T52"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="M53:T53"/>
+    <mergeCell ref="C52:L52"/>
+    <mergeCell ref="C55:L55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9004,8 +9010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:N31"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9146,19 +9152,19 @@
       <c r="C8" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="170" t="s">
+      <c r="D8" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
-      <c r="K8" s="171"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="171"/>
-      <c r="N8" s="172"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="119"/>
       <c r="O8" s="23" t="s">
         <v>145</v>
       </c>
@@ -9495,19 +9501,19 @@
       <c r="C22" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="170" t="s">
+      <c r="D22" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="171"/>
-      <c r="L22" s="171"/>
-      <c r="M22" s="171"/>
-      <c r="N22" s="172"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="119"/>
       <c r="O22" s="73" t="s">
         <v>145</v>
       </c>
@@ -10022,16 +10028,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D27:N27"/>
-    <mergeCell ref="D28:N28"/>
-    <mergeCell ref="D29:N29"/>
-    <mergeCell ref="D30:N30"/>
-    <mergeCell ref="D31:N31"/>
-    <mergeCell ref="D22:N22"/>
-    <mergeCell ref="D23:N23"/>
-    <mergeCell ref="D24:N24"/>
-    <mergeCell ref="D25:N25"/>
-    <mergeCell ref="D26:N26"/>
     <mergeCell ref="D13:N13"/>
     <mergeCell ref="M45:O45"/>
     <mergeCell ref="D34:N34"/>
@@ -10048,6 +10044,16 @@
     <mergeCell ref="D33:N33"/>
     <mergeCell ref="D36:N36"/>
     <mergeCell ref="D35:N35"/>
+    <mergeCell ref="D22:N22"/>
+    <mergeCell ref="D23:N23"/>
+    <mergeCell ref="D24:N24"/>
+    <mergeCell ref="D25:N25"/>
+    <mergeCell ref="D26:N26"/>
+    <mergeCell ref="D27:N27"/>
+    <mergeCell ref="D28:N28"/>
+    <mergeCell ref="D29:N29"/>
+    <mergeCell ref="D30:N30"/>
+    <mergeCell ref="D31:N31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10267,7 +10273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -10487,137 +10493,137 @@
       <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="96" t="s">
         <v>356</v>
       </c>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="96" t="s">
         <v>224</v>
       </c>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="104"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
@@ -10750,10 +10756,10 @@
       <c r="H31" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="96" t="s">
+      <c r="I31" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="97"/>
+      <c r="J31" s="98"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="69" t="s">
@@ -10768,72 +10774,67 @@
       <c r="H32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I32" s="96" t="s">
+      <c r="I32" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="J32" s="97"/>
+      <c r="J32" s="98"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="100"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="101"/>
       <c r="H33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="96" t="s">
+      <c r="I33" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="J33" s="97"/>
+      <c r="J33" s="98"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="98" t="s">
+      <c r="C34" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="100"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="101"/>
       <c r="H34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="96" t="s">
+      <c r="I34" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="J34" s="97"/>
+      <c r="J34" s="98"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="101" t="s">
+      <c r="C35" s="102" t="s">
         <v>223</v>
       </c>
-      <c r="D35" s="102"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="104"/>
       <c r="H35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="96" t="s">
+      <c r="I35" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="97"/>
+      <c r="J35" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C10:L10"/>
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="C34:F34"/>
     <mergeCell ref="C35:F35"/>
@@ -10849,6 +10850,11 @@
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10902,218 +10908,218 @@
       <c r="F11" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="112"/>
+      <c r="G11" s="111"/>
       <c r="H11" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
-      <c r="L11" s="111"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="111"/>
-      <c r="O11" s="111"/>
-      <c r="P11" s="111"/>
-      <c r="Q11" s="111"/>
-      <c r="R11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="112"/>
+      <c r="N11" s="112"/>
+      <c r="O11" s="112"/>
+      <c r="P11" s="112"/>
+      <c r="Q11" s="112"/>
+      <c r="R11" s="111"/>
     </row>
     <row r="12" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E12" s="88" t="s">
         <v>482</v>
       </c>
-      <c r="F12" s="101">
+      <c r="F12" s="102">
         <v>1</v>
       </c>
-      <c r="G12" s="103"/>
-      <c r="H12" s="101" t="s">
+      <c r="G12" s="104"/>
+      <c r="H12" s="102" t="s">
         <v>533</v>
       </c>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
-      <c r="P12" s="102"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="103"/>
+      <c r="L12" s="103"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="103"/>
+      <c r="O12" s="103"/>
+      <c r="P12" s="103"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="104"/>
     </row>
     <row r="13" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E13" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="102" t="s">
         <v>532</v>
       </c>
-      <c r="G13" s="103"/>
-      <c r="H13" s="101" t="s">
+      <c r="G13" s="104"/>
+      <c r="H13" s="102" t="s">
         <v>534</v>
       </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="104"/>
     </row>
     <row r="14" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E14" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="101" t="s">
+      <c r="F14" s="102" t="s">
         <v>532</v>
       </c>
-      <c r="G14" s="103"/>
-      <c r="H14" s="101" t="s">
+      <c r="G14" s="104"/>
+      <c r="H14" s="102" t="s">
         <v>534</v>
       </c>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="102"/>
-      <c r="O14" s="102"/>
-      <c r="P14" s="102"/>
-      <c r="Q14" s="102"/>
-      <c r="R14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="103"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="104"/>
     </row>
     <row r="15" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E15" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="101" t="s">
+      <c r="F15" s="102" t="s">
         <v>532</v>
       </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="101" t="s">
+      <c r="G15" s="104"/>
+      <c r="H15" s="102" t="s">
         <v>535</v>
       </c>
-      <c r="I15" s="102"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="102"/>
-      <c r="O15" s="102"/>
-      <c r="P15" s="102"/>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="103"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="104"/>
     </row>
     <row r="16" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E16" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="101">
+      <c r="F16" s="102">
         <v>3</v>
       </c>
-      <c r="G16" s="103"/>
-      <c r="H16" s="101" t="s">
+      <c r="G16" s="104"/>
+      <c r="H16" s="102" t="s">
         <v>520</v>
       </c>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="103"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="104"/>
     </row>
     <row r="17" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E17" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="101" t="s">
+      <c r="F17" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="G17" s="103"/>
-      <c r="H17" s="101" t="s">
+      <c r="G17" s="104"/>
+      <c r="H17" s="102" t="s">
         <v>521</v>
       </c>
-      <c r="I17" s="102"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="103"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="103"/>
+      <c r="O17" s="103"/>
+      <c r="P17" s="103"/>
+      <c r="Q17" s="103"/>
+      <c r="R17" s="104"/>
     </row>
     <row r="18" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E18" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="G18" s="103"/>
-      <c r="H18" s="101" t="s">
+      <c r="G18" s="104"/>
+      <c r="H18" s="102" t="s">
         <v>522</v>
       </c>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="102"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="102"/>
-      <c r="O18" s="102"/>
-      <c r="P18" s="102"/>
-      <c r="Q18" s="102"/>
-      <c r="R18" s="103"/>
+      <c r="I18" s="103"/>
+      <c r="J18" s="103"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="103"/>
+      <c r="O18" s="103"/>
+      <c r="P18" s="103"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="104"/>
     </row>
     <row r="19" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E19" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="G19" s="103"/>
-      <c r="H19" s="101" t="s">
+      <c r="G19" s="104"/>
+      <c r="H19" s="102" t="s">
         <v>523</v>
       </c>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="102"/>
-      <c r="L19" s="102"/>
-      <c r="M19" s="102"/>
-      <c r="N19" s="102"/>
-      <c r="O19" s="102"/>
-      <c r="P19" s="102"/>
-      <c r="Q19" s="102"/>
-      <c r="R19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="103"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="103"/>
+      <c r="Q19" s="103"/>
+      <c r="R19" s="104"/>
     </row>
     <row r="20" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E20" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="101" t="s">
+      <c r="F20" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="G20" s="103"/>
-      <c r="H20" s="101" t="s">
+      <c r="G20" s="104"/>
+      <c r="H20" s="102" t="s">
         <v>524</v>
       </c>
-      <c r="I20" s="102"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="102"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="102"/>
-      <c r="Q20" s="102"/>
-      <c r="R20" s="103"/>
+      <c r="I20" s="103"/>
+      <c r="J20" s="103"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="104"/>
     </row>
     <row r="25" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E25" s="87" t="s">
@@ -11246,26 +11252,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H16:R16"/>
+    <mergeCell ref="H17:R17"/>
+    <mergeCell ref="H18:R18"/>
+    <mergeCell ref="H19:R19"/>
+    <mergeCell ref="H20:R20"/>
+    <mergeCell ref="H11:R11"/>
+    <mergeCell ref="H12:R12"/>
+    <mergeCell ref="H13:R13"/>
+    <mergeCell ref="H14:R14"/>
+    <mergeCell ref="H15:R15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H11:R11"/>
-    <mergeCell ref="H12:R12"/>
-    <mergeCell ref="H13:R13"/>
-    <mergeCell ref="H14:R14"/>
-    <mergeCell ref="H15:R15"/>
-    <mergeCell ref="H16:R16"/>
-    <mergeCell ref="H17:R17"/>
-    <mergeCell ref="H18:R18"/>
-    <mergeCell ref="H19:R19"/>
-    <mergeCell ref="H20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12369,8 +12375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12472,30 +12478,30 @@
       <c r="E5" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="119"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
       <c r="K5" s="76" t="s">
         <v>469</v>
       </c>
       <c r="M5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="170" t="s">
+      <c r="N5" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="171"/>
-      <c r="P5" s="171"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="171"/>
-      <c r="S5" s="171"/>
-      <c r="T5" s="171"/>
-      <c r="U5" s="171"/>
-      <c r="V5" s="172"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="119"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
@@ -12510,13 +12516,13 @@
       <c r="E6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="120" t="s">
+      <c r="F6" s="167" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="122"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="169"/>
       <c r="K6" s="76" t="s">
         <v>466</v>
       </c>
@@ -12548,13 +12554,13 @@
       <c r="E7" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="123" t="s">
+      <c r="F7" s="170" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="125"/>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="171"/>
+      <c r="J7" s="172"/>
       <c r="K7" s="76" t="s">
         <v>467</v>
       </c>
@@ -12869,21 +12875,21 @@
       <c r="D23" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="160" t="s">
+      <c r="E23" s="123" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="160"/>
-      <c r="G23" s="160"/>
-      <c r="H23" s="160" t="s">
+      <c r="F23" s="123"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="I23" s="160"/>
-      <c r="J23" s="160"/>
-      <c r="K23" s="155" t="s">
+      <c r="I23" s="123"/>
+      <c r="J23" s="123"/>
+      <c r="K23" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="156"/>
-      <c r="M23" s="156"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="28"/>
@@ -12893,25 +12899,25 @@
       <c r="D24" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="157" t="s">
+      <c r="E24" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="158"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="135" t="s">
+      <c r="F24" s="121"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="125" t="s">
         <v>122</v>
       </c>
-      <c r="I24" s="136"/>
-      <c r="J24" s="137"/>
-      <c r="K24" s="150" t="s">
+      <c r="I24" s="126"/>
+      <c r="J24" s="127"/>
+      <c r="K24" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="150"/>
-      <c r="M24" s="150"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="150"/>
-      <c r="P24" s="150"/>
-      <c r="Q24" s="150"/>
+      <c r="L24" s="124"/>
+      <c r="M24" s="124"/>
+      <c r="N24" s="124"/>
+      <c r="O24" s="124"/>
+      <c r="P24" s="124"/>
+      <c r="Q24" s="124"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="29" t="s">
@@ -12923,23 +12929,23 @@
       <c r="D25" s="27">
         <v>5</v>
       </c>
-      <c r="E25" s="157" t="s">
+      <c r="E25" s="120" t="s">
         <v>125</v>
       </c>
-      <c r="F25" s="158"/>
-      <c r="G25" s="159"/>
-      <c r="H25" s="138"/>
-      <c r="I25" s="139"/>
-      <c r="J25" s="140"/>
-      <c r="K25" s="150" t="s">
+      <c r="F25" s="121"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="124" t="s">
         <v>132</v>
       </c>
-      <c r="L25" s="150"/>
-      <c r="M25" s="150"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="150"/>
-      <c r="P25" s="150"/>
-      <c r="Q25" s="150"/>
+      <c r="L25" s="124"/>
+      <c r="M25" s="124"/>
+      <c r="N25" s="124"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="124"/>
+      <c r="Q25" s="124"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="30"/>
@@ -12949,23 +12955,23 @@
       <c r="D26" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="157" t="s">
+      <c r="E26" s="120" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="158"/>
-      <c r="G26" s="159"/>
-      <c r="H26" s="141"/>
-      <c r="I26" s="142"/>
-      <c r="J26" s="143"/>
-      <c r="K26" s="150" t="s">
+      <c r="F26" s="121"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="133"/>
+      <c r="K26" s="124" t="s">
         <v>131</v>
       </c>
-      <c r="L26" s="150"/>
-      <c r="M26" s="150"/>
-      <c r="N26" s="150"/>
-      <c r="O26" s="150"/>
-      <c r="P26" s="150"/>
-      <c r="Q26" s="150"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="29"/>
@@ -12975,25 +12981,25 @@
       <c r="D27" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="135" t="s">
+      <c r="E27" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="136"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="161" t="s">
+      <c r="F27" s="126"/>
+      <c r="G27" s="127"/>
+      <c r="H27" s="134" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="162"/>
-      <c r="J27" s="163"/>
-      <c r="K27" s="150" t="s">
+      <c r="I27" s="135"/>
+      <c r="J27" s="136"/>
+      <c r="K27" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="150"/>
-      <c r="M27" s="150"/>
-      <c r="N27" s="150"/>
-      <c r="O27" s="150"/>
-      <c r="P27" s="150"/>
-      <c r="Q27" s="150"/>
+      <c r="L27" s="124"/>
+      <c r="M27" s="124"/>
+      <c r="N27" s="124"/>
+      <c r="O27" s="124"/>
+      <c r="P27" s="124"/>
+      <c r="Q27" s="124"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="29" t="s">
@@ -13005,21 +13011,21 @@
       <c r="D28" s="27">
         <v>5</v>
       </c>
-      <c r="E28" s="138"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="165"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="150" t="s">
+      <c r="E28" s="128"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="138"/>
+      <c r="J28" s="139"/>
+      <c r="K28" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="L28" s="150"/>
-      <c r="M28" s="150"/>
-      <c r="N28" s="150"/>
-      <c r="O28" s="150"/>
-      <c r="P28" s="150"/>
-      <c r="Q28" s="150"/>
+      <c r="L28" s="124"/>
+      <c r="M28" s="124"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
@@ -13029,24 +13035,24 @@
       <c r="D29" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="141"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="167"/>
-      <c r="I29" s="168"/>
-      <c r="J29" s="169"/>
-      <c r="K29" s="150" t="s">
+      <c r="E29" s="131"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="133"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="141"/>
+      <c r="J29" s="142"/>
+      <c r="K29" s="124" t="s">
         <v>135</v>
       </c>
-      <c r="L29" s="150"/>
-      <c r="M29" s="150"/>
-      <c r="N29" s="150"/>
-      <c r="O29" s="150"/>
-      <c r="P29" s="150"/>
-      <c r="Q29" s="150"/>
+      <c r="L29" s="124"/>
+      <c r="M29" s="124"/>
+      <c r="N29" s="124"/>
+      <c r="O29" s="124"/>
+      <c r="P29" s="124"/>
+      <c r="Q29" s="124"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="132" t="s">
+      <c r="B30" s="149" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -13055,76 +13061,76 @@
       <c r="D30" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="135" t="s">
+      <c r="E30" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="136"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="135" t="s">
+      <c r="F30" s="126"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="125" t="s">
         <v>110</v>
       </c>
-      <c r="I30" s="136"/>
-      <c r="J30" s="137"/>
-      <c r="K30" s="150" t="s">
+      <c r="I30" s="126"/>
+      <c r="J30" s="127"/>
+      <c r="K30" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L30" s="150"/>
-      <c r="M30" s="150"/>
-      <c r="N30" s="150"/>
-      <c r="O30" s="150"/>
-      <c r="P30" s="150"/>
-      <c r="Q30" s="150"/>
+      <c r="L30" s="124"/>
+      <c r="M30" s="124"/>
+      <c r="N30" s="124"/>
+      <c r="O30" s="124"/>
+      <c r="P30" s="124"/>
+      <c r="Q30" s="124"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="133"/>
+      <c r="B31" s="150"/>
       <c r="C31" s="15" t="s">
         <v>115</v>
       </c>
       <c r="D31" s="27">
         <v>5</v>
       </c>
-      <c r="E31" s="138"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="139"/>
-      <c r="J31" s="140"/>
-      <c r="K31" s="150" t="s">
+      <c r="E31" s="128"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="130"/>
+      <c r="K31" s="124" t="s">
         <v>132</v>
       </c>
-      <c r="L31" s="150"/>
-      <c r="M31" s="150"/>
-      <c r="N31" s="150"/>
-      <c r="O31" s="150"/>
-      <c r="P31" s="150"/>
-      <c r="Q31" s="150"/>
+      <c r="L31" s="124"/>
+      <c r="M31" s="124"/>
+      <c r="N31" s="124"/>
+      <c r="O31" s="124"/>
+      <c r="P31" s="124"/>
+      <c r="Q31" s="124"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="134"/>
+      <c r="B32" s="151"/>
       <c r="C32" s="15" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="141"/>
-      <c r="F32" s="142"/>
-      <c r="G32" s="143"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="142"/>
-      <c r="J32" s="143"/>
-      <c r="K32" s="150" t="s">
+      <c r="E32" s="131"/>
+      <c r="F32" s="132"/>
+      <c r="G32" s="133"/>
+      <c r="H32" s="131"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="133"/>
+      <c r="K32" s="124" t="s">
         <v>135</v>
       </c>
-      <c r="L32" s="150"/>
-      <c r="M32" s="150"/>
-      <c r="N32" s="150"/>
-      <c r="O32" s="150"/>
-      <c r="P32" s="150"/>
-      <c r="Q32" s="150"/>
+      <c r="L32" s="124"/>
+      <c r="M32" s="124"/>
+      <c r="N32" s="124"/>
+      <c r="O32" s="124"/>
+      <c r="P32" s="124"/>
+      <c r="Q32" s="124"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="149" t="s">
         <v>92</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -13133,143 +13139,143 @@
       <c r="D33" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="135" t="s">
+      <c r="E33" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="136"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="135" t="s">
+      <c r="F33" s="126"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="125" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="136"/>
-      <c r="J33" s="137"/>
-      <c r="K33" s="150" t="s">
+      <c r="I33" s="126"/>
+      <c r="J33" s="127"/>
+      <c r="K33" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="150"/>
-      <c r="M33" s="150"/>
-      <c r="N33" s="150"/>
-      <c r="O33" s="150"/>
-      <c r="P33" s="150"/>
-      <c r="Q33" s="150"/>
+      <c r="L33" s="124"/>
+      <c r="M33" s="124"/>
+      <c r="N33" s="124"/>
+      <c r="O33" s="124"/>
+      <c r="P33" s="124"/>
+      <c r="Q33" s="124"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="133"/>
+      <c r="B34" s="150"/>
       <c r="C34" s="15" t="s">
         <v>115</v>
       </c>
       <c r="D34" s="27">
         <v>5</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="139"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="138"/>
-      <c r="I34" s="139"/>
-      <c r="J34" s="140"/>
-      <c r="K34" s="150" t="s">
+      <c r="E34" s="128"/>
+      <c r="F34" s="129"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="130"/>
+      <c r="K34" s="124" t="s">
         <v>136</v>
       </c>
-      <c r="L34" s="150"/>
-      <c r="M34" s="150"/>
-      <c r="N34" s="150"/>
-      <c r="O34" s="150"/>
-      <c r="P34" s="150"/>
-      <c r="Q34" s="150"/>
+      <c r="L34" s="124"/>
+      <c r="M34" s="124"/>
+      <c r="N34" s="124"/>
+      <c r="O34" s="124"/>
+      <c r="P34" s="124"/>
+      <c r="Q34" s="124"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="134"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="15" t="s">
         <v>113</v>
       </c>
       <c r="D35" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="141"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="143"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="142"/>
-      <c r="J35" s="143"/>
-      <c r="K35" s="151" t="s">
+      <c r="E35" s="131"/>
+      <c r="F35" s="132"/>
+      <c r="G35" s="133"/>
+      <c r="H35" s="131"/>
+      <c r="I35" s="132"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="143" t="s">
         <v>207</v>
       </c>
-      <c r="L35" s="151"/>
-      <c r="M35" s="151"/>
-      <c r="N35" s="151"/>
-      <c r="O35" s="151"/>
-      <c r="P35" s="151"/>
-      <c r="Q35" s="151"/>
+      <c r="L35" s="143"/>
+      <c r="M35" s="143"/>
+      <c r="N35" s="143"/>
+      <c r="O35" s="143"/>
+      <c r="P35" s="143"/>
+      <c r="Q35" s="143"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B36" s="132" t="s">
+      <c r="B36" s="149" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="144" t="s">
+      <c r="C36" s="158" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="147" t="s">
+      <c r="D36" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="135" t="s">
+      <c r="E36" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="136"/>
-      <c r="G36" s="137"/>
-      <c r="H36" s="135" t="s">
+      <c r="F36" s="126"/>
+      <c r="G36" s="127"/>
+      <c r="H36" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-      <c r="K36" s="152" t="s">
+      <c r="I36" s="126"/>
+      <c r="J36" s="126"/>
+      <c r="K36" s="144" t="s">
         <v>208</v>
       </c>
-      <c r="L36" s="153"/>
-      <c r="M36" s="153"/>
-      <c r="N36" s="153"/>
-      <c r="O36" s="153"/>
-      <c r="P36" s="153"/>
-      <c r="Q36" s="154"/>
+      <c r="L36" s="145"/>
+      <c r="M36" s="145"/>
+      <c r="N36" s="145"/>
+      <c r="O36" s="145"/>
+      <c r="P36" s="145"/>
+      <c r="Q36" s="146"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B37" s="133"/>
-      <c r="C37" s="145"/>
-      <c r="D37" s="148"/>
-      <c r="E37" s="138"/>
-      <c r="F37" s="139"/>
-      <c r="G37" s="140"/>
-      <c r="H37" s="138"/>
-      <c r="I37" s="139"/>
-      <c r="J37" s="139"/>
-      <c r="K37" s="126" t="s">
+      <c r="B37" s="150"/>
+      <c r="C37" s="159"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="128"/>
+      <c r="F37" s="129"/>
+      <c r="G37" s="130"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
+      <c r="K37" s="152" t="s">
         <v>340</v>
       </c>
-      <c r="L37" s="127"/>
-      <c r="M37" s="127"/>
-      <c r="N37" s="127"/>
-      <c r="O37" s="127"/>
-      <c r="P37" s="127"/>
-      <c r="Q37" s="128"/>
+      <c r="L37" s="153"/>
+      <c r="M37" s="153"/>
+      <c r="N37" s="153"/>
+      <c r="O37" s="153"/>
+      <c r="P37" s="153"/>
+      <c r="Q37" s="154"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B38" s="134"/>
-      <c r="C38" s="146"/>
-      <c r="D38" s="149"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="142"/>
-      <c r="J38" s="142"/>
-      <c r="K38" s="129" t="s">
+      <c r="B38" s="151"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="131"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="133"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="132"/>
+      <c r="J38" s="132"/>
+      <c r="K38" s="155" t="s">
         <v>443</v>
       </c>
-      <c r="L38" s="130"/>
-      <c r="M38" s="130"/>
-      <c r="N38" s="130"/>
-      <c r="O38" s="130"/>
-      <c r="P38" s="130"/>
-      <c r="Q38" s="131"/>
+      <c r="L38" s="156"/>
+      <c r="M38" s="156"/>
+      <c r="N38" s="156"/>
+      <c r="O38" s="156"/>
+      <c r="P38" s="156"/>
+      <c r="Q38" s="157"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -13296,20 +13302,28 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="N10:V10"/>
-    <mergeCell ref="N5:V5"/>
-    <mergeCell ref="N6:V6"/>
-    <mergeCell ref="N7:V7"/>
-    <mergeCell ref="N8:V8"/>
-    <mergeCell ref="N9:V9"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="K27:Q27"/>
-    <mergeCell ref="H24:J26"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H27:J29"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K37:Q37"/>
+    <mergeCell ref="K38:Q38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="E36:G38"/>
+    <mergeCell ref="H36:J38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="H30:J32"/>
+    <mergeCell ref="E27:G29"/>
+    <mergeCell ref="E30:G32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E33:G35"/>
+    <mergeCell ref="H33:J35"/>
+    <mergeCell ref="B30:B32"/>
     <mergeCell ref="K33:Q33"/>
     <mergeCell ref="K34:Q34"/>
     <mergeCell ref="K35:Q35"/>
@@ -13323,28 +13337,20 @@
     <mergeCell ref="K30:Q30"/>
     <mergeCell ref="K31:Q31"/>
     <mergeCell ref="K32:Q32"/>
-    <mergeCell ref="H30:J32"/>
-    <mergeCell ref="E27:G29"/>
-    <mergeCell ref="E30:G32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="E33:G35"/>
-    <mergeCell ref="H33:J35"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="K37:Q37"/>
-    <mergeCell ref="K38:Q38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="E36:G38"/>
-    <mergeCell ref="H36:J38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="K27:Q27"/>
+    <mergeCell ref="H24:J26"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H27:J29"/>
+    <mergeCell ref="N10:V10"/>
+    <mergeCell ref="N5:V5"/>
+    <mergeCell ref="N6:V6"/>
+    <mergeCell ref="N7:V7"/>
+    <mergeCell ref="N8:V8"/>
+    <mergeCell ref="N9:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13353,10 +13359,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L15"/>
+  <dimension ref="B3:L23"/>
   <sheetViews>
     <sheetView zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13380,18 +13386,18 @@
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="160" t="s">
+      <c r="C7" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="160"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
-      <c r="L7" s="160"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
@@ -13498,6 +13504,16 @@
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -13518,8 +13534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>